<commit_message>
Programmer String, Number of 1s & other updates.
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oyindamolaakindele/Documents/Techquests/blind-75-leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670E71C0-E0FD-0F4A-9FFF-838258B04202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7D1BE5-2A94-F844-A255-96420EC55EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="17460" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1482,13 +1482,14 @@
   </sheetPr>
   <dimension ref="A1:E1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="2" customWidth="1"/>
     <col min="5" max="5" width="217.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1510,7 +1511,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1527,7 +1528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1544,7 +1545,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
@@ -1561,7 +1562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
@@ -1578,7 +1579,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>20</v>
       </c>
@@ -1595,7 +1596,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
@@ -1612,7 +1613,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>28</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>32</v>
       </c>
@@ -1646,7 +1647,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>36</v>
       </c>
@@ -1663,7 +1664,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>40</v>
       </c>
@@ -1680,7 +1681,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>44</v>
       </c>
@@ -1697,7 +1698,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>48</v>
       </c>
@@ -1714,7 +1715,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>53</v>
       </c>
@@ -1731,7 +1732,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>57</v>
       </c>
@@ -1748,7 +1749,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>61</v>
       </c>
@@ -1765,7 +1766,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>65</v>
       </c>
@@ -1782,7 +1783,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>69</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>74</v>
       </c>
@@ -1816,7 +1817,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>78</v>
       </c>
@@ -1833,7 +1834,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>82</v>
       </c>
@@ -1850,7 +1851,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>86</v>
       </c>
@@ -1867,7 +1868,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>90</v>
       </c>
@@ -1884,7 +1885,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>94</v>
       </c>
@@ -1901,7 +1902,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -1918,7 +1919,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -1935,7 +1936,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>106</v>
       </c>
@@ -1952,7 +1953,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>110</v>
       </c>
@@ -1969,7 +1970,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>114</v>
       </c>
@@ -1986,7 +1987,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>119</v>
       </c>
@@ -2003,7 +2004,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>123</v>
       </c>
@@ -2020,7 +2021,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>127</v>
       </c>
@@ -2037,7 +2038,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>131</v>
       </c>
@@ -2054,7 +2055,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
         <v>135</v>
       </c>
@@ -2071,7 +2072,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
         <v>139</v>
       </c>
@@ -2088,7 +2089,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
         <v>143</v>
       </c>
@@ -2105,7 +2106,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>147</v>
       </c>
@@ -2122,7 +2123,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>152</v>
       </c>
@@ -2139,7 +2140,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>156</v>
       </c>
@@ -2156,7 +2157,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>160</v>
       </c>
@@ -2173,7 +2174,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
         <v>164</v>
       </c>
@@ -2190,7 +2191,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>168</v>
       </c>
@@ -2207,7 +2208,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>173</v>
       </c>
@@ -2224,7 +2225,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>177</v>
       </c>
@@ -2241,7 +2242,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>181</v>
       </c>
@@ -2258,7 +2259,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>185</v>
       </c>
@@ -2275,7 +2276,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>189</v>
       </c>
@@ -2292,7 +2293,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>193</v>
       </c>
@@ -2309,7 +2310,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>198</v>
       </c>
@@ -2326,7 +2327,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>202</v>
       </c>
@@ -2343,7 +2344,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
         <v>206</v>
       </c>
@@ -2360,7 +2361,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>210</v>
       </c>
@@ -2377,7 +2378,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
         <v>215</v>
       </c>
@@ -2394,7 +2395,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
         <v>219</v>
       </c>
@@ -2411,7 +2412,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
         <v>223</v>
       </c>
@@ -2428,7 +2429,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
         <v>227</v>
       </c>
@@ -2445,7 +2446,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
         <v>231</v>
       </c>
@@ -2462,7 +2463,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
         <v>235</v>
       </c>
@@ -2479,7 +2480,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>239</v>
       </c>
@@ -2496,7 +2497,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
         <v>243</v>
       </c>
@@ -2513,7 +2514,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="21" t="s">
         <v>247</v>
       </c>

</xml_diff>